<commit_message>
added edge results - node WASM on mincut still missing
</commit_message>
<xml_diff>
--- a/stats/Performance_paper_sheet_20180203.xlsx
+++ b/stats/Performance_paper_sheet_20180203.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernd Malle\develop\wasm-experiments\stats\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="14295" windowHeight="15060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14295" windowHeight="15060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>RESULTS</t>
   </si>
@@ -119,14 +124,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -140,159 +139,8 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="39">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,194 +183,8 @@
         <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -545,252 +207,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="14">
@@ -837,57 +257,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
-    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
-    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
-    <cellStyle name="Title" xfId="40" builtinId="15"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
-    <cellStyle name="Comma" xfId="46" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
-    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
@@ -957,6 +330,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -965,7 +346,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="414C51"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -1217,24 +598,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.87333333333333" customWidth="1"/>
-    <col min="2" max="2" width="15.7133333333333" customWidth="1"/>
-    <col min="3" max="12" width="8.71333333333333" customWidth="1"/>
-    <col min="13" max="13" width="16.2866666666667" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="12" width="8.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
     <col min="14" max="1025" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" customHeight="1" spans="2:13">
+    <row r="1" spans="2:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
@@ -1248,7 +628,7 @@
       <c r="L1"/>
       <c r="M1"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="42.2" customHeight="1" spans="2:12">
+    <row r="2" spans="2:13" s="1" customFormat="1" ht="42.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1283,7 +663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
+    <row r="3" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1318,7 +698,7 @@
         <v>65227</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
+    <row r="4" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1353,7 +733,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
+    <row r="5" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1388,7 +768,7 @@
         <v>119323</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
+    <row r="6" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
@@ -1417,7 +797,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
+    <row r="7" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1452,7 +832,7 @@
         <v>120450</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
+    <row r="8" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
@@ -1487,7 +867,7 @@
         <v>112353</v>
       </c>
     </row>
-    <row r="9" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
+    <row r="9" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
@@ -1522,7 +902,7 @@
         <v>117550</v>
       </c>
     </row>
-    <row r="10" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
+    <row r="10" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
@@ -1557,17 +937,31 @@
         <v>108537</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
+    <row r="11" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="13"/>
+      <c r="C11" s="5">
+        <v>29</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1670</v>
+      </c>
+      <c r="E11" s="7">
+        <v>545</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1701</v>
+      </c>
+      <c r="G11" s="7">
+        <v>501</v>
+      </c>
+      <c r="H11" s="7">
+        <v>378</v>
+      </c>
+      <c r="I11" s="13">
+        <v>1828</v>
+      </c>
       <c r="J11" s="5">
         <v>987</v>
       </c>
@@ -1578,17 +972,31 @@
         <v>132141</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
+    <row r="12" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="8"/>
+      <c r="C12" s="5">
+        <v>7</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1630</v>
+      </c>
+      <c r="E12" s="7">
+        <v>44</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1570</v>
+      </c>
+      <c r="G12" s="8">
+        <v>245</v>
+      </c>
+      <c r="H12" s="7">
+        <v>328</v>
+      </c>
+      <c r="I12" s="8">
+        <v>1642</v>
+      </c>
       <c r="J12" s="5">
         <v>1106</v>
       </c>
@@ -1599,44 +1007,42 @@
         <v>148301</v>
       </c>
     </row>
-    <row r="21" ht="17.1" customHeight="1"/>
+    <row r="21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <pageMargins left="0.697916666666667" right="0.697916666666667" top="0.75" bottom="0.75" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageMargins left="0.69791666666666696" right="0.69791666666666696" top="0.75" bottom="0.75" header="0.51111111111111096" footer="0.51111111111111096"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1025" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>25</v>
       </c>
@@ -1644,7 +1050,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>27</v>
       </c>
@@ -1652,7 +1058,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>29</v>
       </c>
@@ -1660,7 +1066,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>31</v>
       </c>
@@ -1669,8 +1075,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.698611111111111" right="0.698611111111111" top="0.75" bottom="0.75" header="0.511111111111111" footer="0.511111111111111"/>
-  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter/>
+  <pageMargins left="0.69861111111111096" right="0.69861111111111096" top="0.75" bottom="0.75" header="0.51111111111111096" footer="0.51111111111111096"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adapted output plots - almost perfect now
</commit_message>
<xml_diff>
--- a/stats/Performance_paper_sheet_20180203.xlsx
+++ b/stats/Performance_paper_sheet_20180203.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernd Malle\develop\wasm-experiments\stats\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14295" windowHeight="15060" tabRatio="500"/>
+    <workbookView windowWidth="28695" windowHeight="13680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33">
   <si>
     <t>RESULTS</t>
   </si>
@@ -124,8 +119,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -139,13 +140,182 @@
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -155,19 +325,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FF993300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -179,12 +343,198 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7FFF00"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -207,13 +557,255 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -241,26 +833,79 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Comma[0]" xfId="20" builtinId="6"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Currency[0]" xfId="37" builtinId="7"/>
+    <cellStyle name="Heading 1" xfId="38" builtinId="16"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="20% - Accent1" xfId="42" builtinId="30"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="45" builtinId="17"/>
+    <cellStyle name="Comma" xfId="46" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="47" builtinId="23"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
@@ -330,14 +975,6 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -346,7 +983,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="414C51"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -598,23 +1235,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="B1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="12" width="8.7109375" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.85333333333333" customWidth="1"/>
+    <col min="2" max="2" width="15.7133333333333" customWidth="1"/>
+    <col min="3" max="12" width="8.71333333333333" customWidth="1"/>
+    <col min="13" max="13" width="16.2866666666667" customWidth="1"/>
     <col min="14" max="1025" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="2:13">
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
@@ -628,7 +1266,7 @@
       <c r="L1"/>
       <c r="M1"/>
     </row>
-    <row r="2" spans="2:13" s="1" customFormat="1" ht="42.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" s="1" customFormat="1" ht="42.2" customHeight="1" spans="2:12">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -663,7 +1301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
@@ -691,14 +1329,14 @@
       <c r="J3" s="5">
         <v>619</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="12">
         <v>11068</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="10">
         <v>65227</v>
       </c>
     </row>
-    <row r="4" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
@@ -711,29 +1349,29 @@
       <c r="E4" s="7">
         <v>156</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="12">
         <v>3204.7</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="13">
         <v>3475.8</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="14">
         <v>827.2</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="14">
         <v>3698</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
       <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
@@ -758,7 +1396,7 @@
       <c r="I5" s="7">
         <v>1297</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="12">
         <v>1143</v>
       </c>
       <c r="K5" s="5">
@@ -768,7 +1406,7 @@
         <v>119323</v>
       </c>
     </row>
-    <row r="6" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
@@ -793,11 +1431,17 @@
       <c r="I6" s="7">
         <v>1133</v>
       </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
       <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
@@ -832,17 +1476,17 @@
         <v>120450</v>
       </c>
     </row>
-    <row r="8" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
       <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="9">
         <v>4</v>
       </c>
       <c r="D8" s="7">
         <v>730</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="9">
         <v>44</v>
       </c>
       <c r="F8" s="7">
@@ -851,7 +1495,7 @@
       <c r="G8" s="7">
         <v>352</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="9">
         <v>272</v>
       </c>
       <c r="I8" s="7">
@@ -867,7 +1511,7 @@
         <v>112353</v>
       </c>
     </row>
-    <row r="9" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
       <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
@@ -902,17 +1546,17 @@
         <v>117550</v>
       </c>
     </row>
-    <row r="10" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
       <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="10">
         <v>3</v>
       </c>
       <c r="D10" s="7">
         <v>780</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="10">
         <v>43</v>
       </c>
       <c r="F10" s="7">
@@ -921,33 +1565,33 @@
       <c r="G10" s="7">
         <v>147</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="10">
         <v>179</v>
       </c>
       <c r="I10" s="7">
         <v>896</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="6">
         <v>610</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="6">
         <v>2074</v>
       </c>
       <c r="L10" s="5">
         <v>108537</v>
       </c>
     </row>
-    <row r="11" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
       <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="11">
         <v>29</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="11">
         <v>1670</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="11">
         <v>545</v>
       </c>
       <c r="F11" s="7">
@@ -959,7 +1603,7 @@
       <c r="H11" s="7">
         <v>378</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="7">
         <v>1828</v>
       </c>
       <c r="J11" s="5">
@@ -972,7 +1616,7 @@
         <v>132141</v>
       </c>
     </row>
-    <row r="12" spans="2:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" s="1" customFormat="1" ht="34.5" customHeight="1" spans="2:12">
       <c r="B12" s="4" t="s">
         <v>21</v>
       </c>
@@ -1003,46 +1647,48 @@
       <c r="K12" s="5">
         <v>3666</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="12">
         <v>148301</v>
       </c>
     </row>
-    <row r="21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="17.1" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.69791666666666696" right="0.69791666666666696" top="0.75" bottom="0.75" header="0.51111111111111096" footer="0.51111111111111096"/>
+  <pageMargins left="0.697916666666667" right="0.697916666666667" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1025" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2">
       <c r="B2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3">
       <c r="B6" t="s">
         <v>25</v>
       </c>
@@ -1050,7 +1696,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3">
       <c r="B7" t="s">
         <v>27</v>
       </c>
@@ -1058,7 +1704,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3">
       <c r="B8" t="s">
         <v>29</v>
       </c>
@@ -1066,7 +1712,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3">
       <c r="B9" t="s">
         <v>31</v>
       </c>
@@ -1075,7 +1721,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.69861111111111096" right="0.69861111111111096" top="0.75" bottom="0.75" header="0.51111111111111096" footer="0.51111111111111096"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.697916666666667" right="0.697916666666667" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
+  <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>